<commit_message>
Worked on commands and restructured
</commit_message>
<xml_diff>
--- a/book_rental/management/commands/uploads/book_list.xlsx
+++ b/book_rental/management/commands/uploads/book_list.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="62">
   <si>
     <t>Code</t>
   </si>
@@ -91,7 +91,7 @@
     <t>PC-000001</t>
   </si>
   <si>
-    <t>BP-000025</t>
+    <t>BP-00001</t>
   </si>
   <si>
     <t>1238765398756.jpg</t>
@@ -103,7 +103,7 @@
     <t>Computer, CSE, Science</t>
   </si>
   <si>
-    <t>A-000159</t>
+    <t>A-000001</t>
   </si>
   <si>
     <t>Introduction to Computer Science2</t>
@@ -118,7 +118,7 @@
     <t>1238765398757.jpg</t>
   </si>
   <si>
-    <t>A-000160</t>
+    <t>A-000002</t>
   </si>
   <si>
     <t>Introduction to Computer Science3</t>
@@ -127,7 +127,7 @@
     <t>1238765398758</t>
   </si>
   <si>
-    <t>A-000159, A-000160, A-000161</t>
+    <t>A-000001,A-000002,A-000003</t>
   </si>
   <si>
     <t>Introduction to Computer Science4</t>
@@ -152,6 +152,9 @@
   </si>
   <si>
     <t>1238765398755</t>
+  </si>
+  <si>
+    <t>A-000004,A-000005,A-000006</t>
   </si>
   <si>
     <t>Introduction to Computer Science7</t>
@@ -299,6 +302,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
+    <col customWidth="1" min="2" max="2" width="54.14"/>
     <col customWidth="1" min="7" max="10" width="15.0"/>
     <col customWidth="1" min="11" max="11" width="11.43"/>
     <col customWidth="1" min="15" max="15" width="19.0"/>
@@ -593,7 +597,7 @@
         <v>29</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="S5" s="1">
         <v>1.0</v>
@@ -642,7 +646,7 @@
         <v>29</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="S6" s="1">
         <v>1.0</v>
@@ -691,7 +695,7 @@
         <v>29</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="S7" s="1">
         <v>1.0</v>
@@ -702,7 +706,7 @@
     </row>
     <row r="8">
       <c r="B8" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2" t="s">
@@ -710,7 +714,7 @@
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>24</v>
@@ -718,7 +722,7 @@
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
       <c r="J8" s="6" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K8" s="1">
         <v>3.0</v>
@@ -742,7 +746,7 @@
         <v>29</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="S8" s="1">
         <v>1.0</v>
@@ -753,7 +757,7 @@
     </row>
     <row r="9">
       <c r="B9" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2" t="s">
@@ -761,7 +765,7 @@
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>24</v>
@@ -769,7 +773,7 @@
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
       <c r="J9" s="6" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K9" s="1">
         <v>1.0</v>
@@ -793,7 +797,7 @@
         <v>29</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="S9" s="1">
         <v>1.0</v>
@@ -804,7 +808,7 @@
     </row>
     <row r="10">
       <c r="B10" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2" t="s">
@@ -812,7 +816,7 @@
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>24</v>
@@ -844,7 +848,7 @@
         <v>29</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="S10" s="1">
         <v>1.0</v>
@@ -855,7 +859,7 @@
     </row>
     <row r="11">
       <c r="B11" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
@@ -863,7 +867,7 @@
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>24</v>
@@ -895,7 +899,7 @@
         <v>29</v>
       </c>
       <c r="R11" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="S11" s="1">
         <v>1.0</v>
@@ -906,7 +910,7 @@
     </row>
     <row r="12">
       <c r="B12" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2" t="s">
@@ -914,7 +918,7 @@
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>24</v>
@@ -946,7 +950,7 @@
         <v>29</v>
       </c>
       <c r="R12" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="S12" s="1">
         <v>1.0</v>
@@ -957,7 +961,7 @@
     </row>
     <row r="13">
       <c r="B13" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
@@ -965,7 +969,7 @@
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>24</v>
@@ -997,7 +1001,7 @@
         <v>29</v>
       </c>
       <c r="R13" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="S13" s="1">
         <v>1.0</v>
@@ -1008,7 +1012,7 @@
     </row>
     <row r="14">
       <c r="B14" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
@@ -1016,7 +1020,7 @@
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>24</v>
@@ -1048,7 +1052,7 @@
         <v>29</v>
       </c>
       <c r="R14" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="S14" s="1">
         <v>1.0</v>
@@ -1059,7 +1063,7 @@
     </row>
     <row r="15">
       <c r="B15" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2" t="s">
@@ -1067,7 +1071,7 @@
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>24</v>
@@ -1099,7 +1103,7 @@
         <v>29</v>
       </c>
       <c r="R15" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="S15" s="1">
         <v>1.0</v>
@@ -1110,7 +1114,7 @@
     </row>
     <row r="16">
       <c r="B16" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2" t="s">
@@ -1118,7 +1122,7 @@
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>24</v>
@@ -1126,7 +1130,7 @@
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
       <c r="J16" s="6" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K16" s="1">
         <v>3.0</v>
@@ -1150,7 +1154,7 @@
         <v>29</v>
       </c>
       <c r="R16" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="S16" s="1">
         <v>1.0</v>
@@ -1161,7 +1165,7 @@
     </row>
     <row r="17">
       <c r="B17" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2" t="s">
@@ -1169,7 +1173,7 @@
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>24</v>
@@ -1177,7 +1181,7 @@
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
       <c r="J17" s="6" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K17" s="1">
         <v>1.0</v>
@@ -1201,7 +1205,7 @@
         <v>29</v>
       </c>
       <c r="R17" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="S17" s="1">
         <v>1.0</v>

</xml_diff>